<commit_message>
Updated title of the picture
</commit_message>
<xml_diff>
--- a/draft.xlsx
+++ b/draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vigne\Documents\block_3\DSCI_532\DSCI532_group214_movies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72898F9B-1701-4AEF-B49E-82E3AAC32F35}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3152F486-B61D-4BC5-AF10-1AAB4FD53DD5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{D77099CD-3AFB-440E-B39A-CC8AD4B9794B}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 etc …</t>
   </si>
   <si>
-    <t>Insights from the movies database</t>
+    <t>Movie Profitability Dashboard</t>
   </si>
 </sst>
 </file>
@@ -261,6 +261,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -268,33 +331,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -306,47 +342,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -988,7 +988,7 @@
   <dimension ref="B1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1010,579 +1010,590 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="22"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="6"/>
     </row>
     <row r="3" spans="2:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="23"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="27"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="11"/>
     </row>
     <row r="4" spans="2:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="23"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="28" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="30"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="24"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="27"/>
+      <c r="S4" s="11"/>
     </row>
     <row r="5" spans="2:19" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="23"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="27"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="11"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B6" s="23"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="4" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="4" t="s">
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="27"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="11"/>
     </row>
     <row r="7" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="23"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="27"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="11"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B8" s="23"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="12" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="27"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="11"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B9" s="23"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="27"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="11"/>
     </row>
     <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="23"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="27"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="11"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B11" s="23"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="12" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="27"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="11"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B12" s="23"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="27"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="11"/>
     </row>
     <row r="13" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="23"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="27"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="11"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B14" s="23"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="12" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="27"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="11"/>
     </row>
     <row r="15" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="23"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="8"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="8"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="13"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="10" t="s">
+      <c r="N15" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="27"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="11"/>
     </row>
     <row r="16" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="23"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="27"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="11"/>
     </row>
     <row r="17" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="23"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="12" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="19" t="s">
+      <c r="E17" s="17"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="4" t="s">
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="N17" s="15" t="s">
+      <c r="N17" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="11"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B18" s="23"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="27"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="11"/>
     </row>
     <row r="19" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="23"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="27"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="11"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B20" s="23"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="12" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="27"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="11"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B21" s="23"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="27"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="11"/>
     </row>
     <row r="22" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="23"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="27"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="11"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B23" s="23"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="27"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="11"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B24" s="23"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="27"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="11"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B25" s="23"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="27"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="11"/>
     </row>
     <row r="26" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="23"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="8"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="13"/>
       <c r="M26" s="3"/>
-      <c r="N26" s="10" t="s">
+      <c r="N26" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="27"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="11"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B27" s="23"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="27"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="11"/>
     </row>
     <row r="28" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="26"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D11:E13"/>
+    <mergeCell ref="M17:M25"/>
+    <mergeCell ref="N17:Q25"/>
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="G17:K26"/>
+    <mergeCell ref="H6:K14"/>
+    <mergeCell ref="G6:G14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="M6:M14"/>
+    <mergeCell ref="N6:Q14"/>
+    <mergeCell ref="N15:Q15"/>
     <mergeCell ref="R5:R26"/>
     <mergeCell ref="D27:R27"/>
     <mergeCell ref="F5:Q5"/>
@@ -1599,17 +1610,6 @@
     <mergeCell ref="G4:Q4"/>
     <mergeCell ref="L6:L26"/>
     <mergeCell ref="F6:F26"/>
-    <mergeCell ref="M17:M25"/>
-    <mergeCell ref="N17:Q25"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="G17:K26"/>
-    <mergeCell ref="H6:K14"/>
-    <mergeCell ref="G6:G14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="M6:M14"/>
-    <mergeCell ref="N6:Q14"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="D11:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>